<commit_message>
Adding support for application rename
</commit_message>
<xml_diff>
--- a/Excel Template.xlsx
+++ b/Excel Template.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27425"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27726"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://veracode-my.sharepoint.com/personal/rpereira_veracode_com/Documents/Projects/plugins/Veracode-Bulk-Application-Update/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="19" documentId="11_6C5D155443060114056EE7543FCFA25781696894" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{8C0134D5-E89D-4F00-A541-66D33040E640}"/>
+  <xr:revisionPtr revIDLastSave="23" documentId="11_6C5D155443060114056EE7543FCFA25781696894" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{9BECA18E-E8D6-429C-B9D2-CDC1FD500188}"/>
   <bookViews>
-    <workbookView minimized="1" xWindow="3435" yWindow="1950" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="57480" yWindow="-105" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="43">
   <si>
     <t>Custom fields can be renamed, in that case, you need to put their real name here</t>
   </si>
@@ -143,6 +143,12 @@
   </si>
   <si>
     <t>This template can be used to bulk update applications into the Veracode platform by using the plugin at https://github.com/cadonuno/Veracode-Bulk-Application-Update. Above each field name, there's a description of the allowed values. After execution, a new column will be added with the status of each application</t>
+  </si>
+  <si>
+    <t>Set this field to update the application name</t>
+  </si>
+  <si>
+    <t>New Application Name</t>
   </si>
 </sst>
 </file>
@@ -221,6 +227,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -520,154 +530,160 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AJ2"/>
+  <dimension ref="A1:AK2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L2" sqref="L2"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="34.85546875" customWidth="1"/>
-    <col min="2" max="2" width="17.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="30.42578125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="24.140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="15.5703125" customWidth="1"/>
-    <col min="6" max="6" width="14.28515625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="14.140625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="30.140625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="32.5703125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="20.42578125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="21.85546875" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="17.7109375" customWidth="1"/>
-    <col min="13" max="20" width="8.5703125" bestFit="1" customWidth="1"/>
-    <col min="21" max="36" width="9.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="2" width="34.81640625" customWidth="1"/>
+    <col min="3" max="3" width="17.453125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="30.453125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="24.1796875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="15.54296875" customWidth="1"/>
+    <col min="7" max="7" width="14.26953125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="14.1796875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="30.1796875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="32.54296875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="20.453125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="21.81640625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="17.7265625" customWidth="1"/>
+    <col min="14" max="21" width="8.54296875" bestFit="1" customWidth="1"/>
+    <col min="22" max="37" width="9.54296875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:36" s="1" customFormat="1" ht="130.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:37" s="1" customFormat="1" ht="130.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="B1" s="4" t="s">
+      <c r="B1" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="C1" s="4" t="s">
         <v>38</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="L1" s="3" t="s">
+      <c r="M1" s="3" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:36" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:37" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A2" s="2" t="s">
         <v>39</v>
       </c>
       <c r="B2" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="C2" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="D2" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="D2" s="2" t="s">
+      <c r="E2" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="E2" s="2" t="s">
+      <c r="F2" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="F2" s="2" t="s">
+      <c r="G2" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="G2" s="2" t="s">
+      <c r="H2" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="H2" s="2" t="s">
+      <c r="I2" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="I2" s="2" t="s">
+      <c r="J2" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="J2" s="2" t="s">
+      <c r="K2" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="K2" s="2" t="s">
+      <c r="L2" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="L2" s="2" t="s">
+      <c r="M2" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="M2" s="2" t="s">
+      <c r="N2" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="N2" s="2" t="s">
+      <c r="O2" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="O2" s="2" t="s">
+      <c r="P2" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="P2" s="2" t="s">
+      <c r="Q2" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="Q2" s="2" t="s">
+      <c r="R2" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="R2" s="2" t="s">
+      <c r="S2" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="S2" s="2" t="s">
+      <c r="T2" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="T2" s="2" t="s">
+      <c r="U2" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="U2" s="2" t="s">
+      <c r="V2" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="V2" s="2" t="s">
+      <c r="W2" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="W2" s="2" t="s">
+      <c r="X2" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="X2" s="2" t="s">
+      <c r="Y2" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="Y2" s="2" t="s">
+      <c r="Z2" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="Z2" s="2" t="s">
+      <c r="AA2" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="AA2" s="2" t="s">
+      <c r="AB2" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="AB2" s="2" t="s">
+      <c r="AC2" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="AC2" s="2" t="s">
+      <c r="AD2" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="AD2" s="2" t="s">
+      <c r="AE2" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="AE2" s="2" t="s">
+      <c r="AF2" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="AF2" s="2" t="s">
+      <c r="AG2" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="AG2" s="2" t="s">
+      <c r="AH2" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="AH2" s="2" t="s">
+      <c r="AI2" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="AI2" s="2" t="s">
+      <c r="AJ2" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="AJ2" s="2" t="s">
+      <c r="AK2" s="2" t="s">
         <v>34</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Refactoring to use veracode-api-py instead of manually building requests
</commit_message>
<xml_diff>
--- a/Excel Template.xlsx
+++ b/Excel Template.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27726"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28827"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://veracode-my.sharepoint.com/personal/rpereira_veracode_com/Documents/Projects/plugins/Veracode-Bulk-Application-Update/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rpereira\OneDrive - Veracode\Projects\plugins\Veracode-Bulk-Application-Update\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="23" documentId="11_6C5D155443060114056EE7543FCFA25781696894" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{9BECA18E-E8D6-429C-B9D2-CDC1FD500188}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7AB14AE4-F48C-464E-B7F6-6562EF3AAE0C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="57480" yWindow="-105" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,10 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="43">
-  <si>
-    <t>Custom fields can be renamed, in that case, you need to put their real name here</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="46">
   <si>
     <t>Policy</t>
   </si>
@@ -46,12 +43,6 @@
     <t>Teams</t>
   </si>
   <si>
-    <t>Dynamic Scan Approval</t>
-  </si>
-  <si>
-    <t>Archer Application Name</t>
-  </si>
-  <si>
     <t>Custom 1</t>
   </si>
   <si>
@@ -130,15 +121,9 @@
     <t>Case-sensitive policy name (defaults to the one assigned to the Business Criticality)</t>
   </si>
   <si>
-    <t>Comma-delimited list of teams</t>
-  </si>
-  <si>
     <t>Business Criticality</t>
   </si>
   <si>
-    <t>Mandatory*</t>
-  </si>
-  <si>
     <t>Application Name</t>
   </si>
   <si>
@@ -149,6 +134,30 @@
   </si>
   <si>
     <t>New Application Name</t>
+  </si>
+  <si>
+    <t>To clear, set it to NULL</t>
+  </si>
+  <si>
+    <t>Comma-delimited list of tags - This will replace the current list of tags assigned to the application. To clear the tags, set it to NULL</t>
+  </si>
+  <si>
+    <t>To clear the Business Unit, set it to NULL</t>
+  </si>
+  <si>
+    <t>To clear the Business Owner, set it to NULL</t>
+  </si>
+  <si>
+    <t>To clear the Owner Email, set it to NULL</t>
+  </si>
+  <si>
+    <t>Custom fields can be renamed, in that case, you need to put their real name here. Keeping the original names will throw an error</t>
+  </si>
+  <si>
+    <t>Cannot be cleared</t>
+  </si>
+  <si>
+    <t>Comma-delimited list of teams - This will replace the current list of teams assigned to the application.</t>
   </si>
 </sst>
 </file>
@@ -227,10 +236,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -530,161 +535,168 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AK2"/>
+  <dimension ref="A1:AI2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="J2" sqref="J2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="2" width="34.81640625" customWidth="1"/>
-    <col min="3" max="3" width="17.453125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="30.453125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="24.1796875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="15.54296875" customWidth="1"/>
-    <col min="7" max="7" width="14.26953125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="14.1796875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="30.1796875" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="32.54296875" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="20.453125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="21.81640625" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="17.7265625" customWidth="1"/>
-    <col min="14" max="21" width="8.54296875" bestFit="1" customWidth="1"/>
-    <col min="22" max="37" width="9.54296875" bestFit="1" customWidth="1"/>
+    <col min="1" max="2" width="34.85546875" customWidth="1"/>
+    <col min="3" max="3" width="17.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="30.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="24.140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="15.5703125" customWidth="1"/>
+    <col min="7" max="7" width="14.28515625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="14.140625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="30.140625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="32.5703125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="17.7109375" customWidth="1"/>
+    <col min="12" max="19" width="8.5703125" bestFit="1" customWidth="1"/>
+    <col min="20" max="35" width="9.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:37" s="1" customFormat="1" ht="130.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:35" s="1" customFormat="1" ht="151.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="G1" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="C1" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>35</v>
+      <c r="I1" s="1" t="s">
+        <v>42</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="M1" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="K1" s="3" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="2" spans="1:35" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="D2" s="2" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="2" spans="1:37" s="2" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="D2" s="2" t="s">
+      <c r="E2" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="E2" s="2" t="s">
+      <c r="F2" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="F2" s="2" t="s">
+      <c r="G2" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="G2" s="2" t="s">
+      <c r="H2" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="H2" s="2" t="s">
+      <c r="I2" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="I2" s="2" t="s">
+      <c r="J2" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="J2" s="2" t="s">
+      <c r="K2" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="K2" s="2" t="s">
+      <c r="L2" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="L2" s="2" t="s">
+      <c r="M2" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="M2" s="2" t="s">
+      <c r="N2" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="N2" s="2" t="s">
+      <c r="O2" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="O2" s="2" t="s">
+      <c r="P2" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="P2" s="2" t="s">
+      <c r="Q2" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="Q2" s="2" t="s">
+      <c r="R2" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="R2" s="2" t="s">
+      <c r="S2" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="S2" s="2" t="s">
+      <c r="T2" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="T2" s="2" t="s">
+      <c r="U2" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="U2" s="2" t="s">
+      <c r="V2" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="V2" s="2" t="s">
+      <c r="W2" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="W2" s="2" t="s">
+      <c r="X2" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="X2" s="2" t="s">
+      <c r="Y2" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="Y2" s="2" t="s">
+      <c r="Z2" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="Z2" s="2" t="s">
+      <c r="AA2" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="AA2" s="2" t="s">
+      <c r="AB2" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="AB2" s="2" t="s">
+      <c r="AC2" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="AC2" s="2" t="s">
+      <c r="AD2" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="AD2" s="2" t="s">
+      <c r="AE2" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="AE2" s="2" t="s">
+      <c r="AF2" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="AF2" s="2" t="s">
+      <c r="AG2" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="AG2" s="2" t="s">
+      <c r="AH2" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="AH2" s="2" t="s">
+      <c r="AI2" s="2" t="s">
         <v>31</v>
-      </c>
-      <c r="AI2" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="AJ2" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="AK2" s="2" t="s">
-        <v>34</v>
       </c>
     </row>
   </sheetData>

</xml_diff>